<commit_message>
Handle quotes in hyperlink sheet names in hyperlink adresses (#18568)
If sheet name contains only numbers its enclosing single quotes are removed
Same for sheet names including spaces
Also solves (SHEET-98)
Change-Id: I0ada3e6ff949dd77dc9e852d446a08a1bccf5ccb
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/hyper_links.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/hyper_links.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="2015" sheetId="3" r:id="rId3"/>
+    <sheet name="two words" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>This link goes to google</t>
   </si>
@@ -41,6 +43,12 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Link to B3 on sheet '2015'</t>
+  </si>
+  <si>
+    <t>Link to C3 on sheet 'two words'</t>
   </si>
 </sst>
 </file>
@@ -426,7 +434,7 @@
   <dimension ref="B5:AO164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -449,7 +457,12 @@
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="C9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="2:4">
       <c r="D11" s="1" t="s">
@@ -509,6 +522,8 @@
     <hyperlink ref="D11" r:id="rId3" display="http://google.fi"/>
     <hyperlink ref="AO164" r:id="rId4"/>
     <hyperlink ref="C18" r:id="rId5" tooltip="tooltip text is not address"/>
+    <hyperlink ref="B9" location="'2015'!B3" display="Link to B3 on sheet '2015'"/>
+    <hyperlink ref="C9" location="'two words'!C3" display="Link to C3 on sheet 'two words'"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -549,4 +564,54 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="3:3">
+      <c r="C3">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove hyperlink handler explicit navigator in favor of UI.getCurrent().getNavigator() per recommendation
Also fix unit test that had indirect method reference to a private
method whose signature changed.

Method is now protected so it can be extended/wrapped/exposed by
subclasses, including unit tests.

Changed test to use the new cell/formula based parsing while still
handling the same test cases.
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/hyper_links.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/hyper_links.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregWoolsey\git\spreadsheet\vaadin-spreadsheet\src\test\resources\test_sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E733BCB9-9EA4-4C3A-AF6D-408DA7C4BB85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17535" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,8 +18,13 @@
     <sheet name="2015" sheetId="3" r:id="rId3"/>
     <sheet name="two words" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>This link goes to google</t>
   </si>
@@ -49,12 +60,15 @@
   </si>
   <si>
     <t>Link to C3 on sheet 'two words'</t>
+  </si>
+  <si>
+    <t>#A3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -106,6 +120,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -430,22 +452,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:AO164"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:AO164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.875" customWidth="1"/>
     <col min="41" max="41" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:4" ht="29" customHeight="1">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="str">
+        <f>HYPERLINK(C1, "link to A3 via value of C1")</f>
+        <v>link to A3 via value of C1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>HYPERLINK("https://www.google.com", "link to google via function")</f>
+        <v>link to google via function</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -464,66 +501,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="str">
         <f>HYPERLINK("http://google.com","HYPERLINK FUNCTION google")</f>
         <v>HYPERLINK FUNCTION google</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="str">
         <f>HYPERLINK("#Sheet2!A3","link to A3 on Sheet2")</f>
         <v>link to A3 on Sheet2</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="str">
         <f>HYPERLINK("#Sheet2!A3","link to A3 on Sheet2")</f>
         <v>link to A3 on Sheet2</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="str">
         <f>HYPERLINK(("#A1"), "LINK TO A1 on this sheet")</f>
         <v>LINK TO A1 on this sheet</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D28" s="1" t="str">
         <f>HYPERLINK(("#A1"), "LINK TO A1 on this sheet")</f>
         <v>LINK TO A1 on this sheet</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="str">
         <f>HYPERLINK("[hyper_links.xlsx]Sheet2!B10","link to sheet2 B10")</f>
         <v>link to sheet2 B10</v>
       </c>
     </row>
-    <row r="164" spans="41:41">
+    <row r="164" spans="41:41" x14ac:dyDescent="0.25">
       <c r="AO164" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="http://google.com"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="D11" r:id="rId3" display="http://google.fi"/>
-    <hyperlink ref="AO164" r:id="rId4"/>
-    <hyperlink ref="C18" r:id="rId5" tooltip="tooltip text is not address"/>
-    <hyperlink ref="B9" location="'2015'!B3" display="Link to B3 on sheet '2015'"/>
-    <hyperlink ref="C9" location="'two words'!C3" display="Link to C3 on sheet 'two words'"/>
+    <hyperlink ref="B5" r:id="rId1" display="http://google.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D11" r:id="rId3" display="http://google.fi" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="AO164" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C18" r:id="rId5" tooltip="tooltip text is not address" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B9" location="'2015'!B3" display="Link to B3 on sheet '2015'" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C9" location="'two words'!C3" display="Link to C3 on sheet 'two words'" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -536,22 +573,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:S47"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>5000</f>
         <v>5000</v>
       </c>
     </row>
-    <row r="47" spans="19:19">
+    <row r="47" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S47" t="s">
         <v>6</v>
       </c>
@@ -567,16 +604,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>300</v>
       </c>
@@ -592,16 +629,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:3">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>125</v>
       </c>

</xml_diff>